<commit_message>
DESTROY ALL BUGS. Made our placeholder conference shorter than the number of matches, to force it to shuffle them; fixed an import bug; added a constraint to restrict games in the same match slot, and fixed a bug that kept moves from working. #1140938 #1140946
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -76,7 +76,7 @@
     <t>I</t>
   </si>
   <si>
-    <t>XD 1/12/2014-1/20/2014, XD 3/3/2014</t>
+    <t>XD 1/7/2014-1/14/2014, XD 1/3/2014</t>
   </si>
   <si>
     <t>105-IRISH-WEBSTER 1</t>
@@ -225,7 +225,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -290,19 +290,11 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="8" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="7" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -323,22 +315,7 @@
     <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
     <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF9C0006"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <numFmt formatCode="GENERAL" numFmtId="164"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <sz val="11"/>
@@ -438,10 +415,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="E14" activeCellId="0" pane="topLeft" sqref="E14"/>
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -457,7 +434,7 @@
     <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.72959183673469"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="1">
       <c r="B1" s="1"/>
       <c r="C1" s="2" t="s">
         <v>0</v>
@@ -469,7 +446,7 @@
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.9" outlineLevel="0" r="2">
       <c r="A2" s="5"/>
       <c r="B2" s="6" t="s">
         <v>1</v>
@@ -521,7 +498,7 @@
       <c r="A4" s="11" t="n">
         <v>102</v>
       </c>
-      <c r="B4" s="16"/>
+      <c r="B4" s="12"/>
       <c r="C4" s="15" t="s">
         <v>12</v>
       </c>
@@ -535,16 +512,16 @@
       <c r="G4" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="17" t="s">
+      <c r="H4" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="18"/>
+      <c r="I4" s="17"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="5">
-      <c r="A5" s="19" t="n">
+      <c r="A5" s="11" t="n">
         <v>103</v>
       </c>
-      <c r="B5" s="16"/>
+      <c r="B5" s="12"/>
       <c r="C5" s="15" t="s">
         <v>15</v>
       </c>
@@ -567,7 +544,7 @@
       <c r="A6" s="11" t="n">
         <v>104</v>
       </c>
-      <c r="B6" s="16"/>
+      <c r="B6" s="12"/>
       <c r="C6" s="15" t="s">
         <v>17</v>
       </c>
@@ -575,22 +552,22 @@
       <c r="E6" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="16" t="n">
+      <c r="F6" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="G6" s="16" t="s">
+      <c r="G6" s="12" t="s">
         <v>18</v>
       </c>
       <c r="H6" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="I6" s="18"/>
+      <c r="I6" s="17"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="7">
       <c r="A7" s="11" t="n">
         <v>105</v>
       </c>
-      <c r="B7" s="16"/>
+      <c r="B7" s="12"/>
       <c r="C7" s="15" t="s">
         <v>20</v>
       </c>
@@ -604,10 +581,10 @@
       <c r="G7" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="20" t="s">
+      <c r="H7" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="I7" s="21" t="s">
+      <c r="I7" s="19" t="s">
         <v>22</v>
       </c>
     </row>
@@ -615,7 +592,7 @@
       <c r="A8" s="11" t="n">
         <v>106</v>
       </c>
-      <c r="B8" s="16"/>
+      <c r="B8" s="12"/>
       <c r="C8" s="15" t="s">
         <v>23</v>
       </c>
@@ -632,13 +609,13 @@
       <c r="H8" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="I8" s="18"/>
+      <c r="I8" s="17"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.05" outlineLevel="0" r="9">
       <c r="A9" s="11" t="n">
         <v>107</v>
       </c>
-      <c r="B9" s="16"/>
+      <c r="B9" s="12"/>
       <c r="C9" s="15" t="s">
         <v>24</v>
       </c>
@@ -652,24 +629,20 @@
       <c r="G9" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="18" t="s">
+      <c r="H9" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="I9" s="18"/>
-    </row>
+      <c r="I9" s="17"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.05" outlineLevel="0" r="14"/>
   </sheetData>
   <conditionalFormatting sqref="C1:C2">
     <cfRule aboveAverage="0" bottom="0" dxfId="0" equalAverage="0" operator="duplicateValues" percent="0" priority="2" rank="0" text="" type="duplicateValues">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H5,H8">
+  <conditionalFormatting sqref="C1:C2">
     <cfRule aboveAverage="0" bottom="0" dxfId="1" equalAverage="0" operator="duplicateValues" percent="0" priority="3" rank="0" text="" type="duplicateValues">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C2">
-    <cfRule aboveAverage="0" bottom="0" dxfId="2" equalAverage="0" operator="duplicateValues" percent="0" priority="4" rank="0" text="" type="duplicateValues">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Included conference in the output
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -16,14 +16,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
   <si>
     <t>TEAM  LIST  AS  OF :</t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
     <t>Team</t>
   </si>
   <si>
@@ -97,6 +94,12 @@
   </si>
   <si>
     <t>no 4:40-5:40</t>
+  </si>
+  <si>
+    <t>Team ID</t>
+  </si>
+  <si>
+    <t>Conference #</t>
   </si>
 </sst>
 </file>
@@ -114,14 +117,6 @@
     <font>
       <sz val="11"/>
       <name val="Berlin Sans FB"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="11"/>
-      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -151,6 +146,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <name val="Berlin Sans FB"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -209,31 +211,31 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -633,12 +635,13 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="8.7109375"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31.28515625"/>
     <col min="4" max="4" width="8.7109375"/>
     <col min="5" max="5" width="7.5703125"/>
@@ -662,192 +665,208 @@
       <c r="I1" s="4"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="5"/>
-      <c r="B2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="7" t="s">
+      <c r="A2" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="F2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="G2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="H2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="I2" s="8" t="s">
         <v>7</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="11">
+      <c r="A3" s="9">
         <v>101</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="13" t="s">
+      <c r="B3" s="10">
+        <v>1</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="12"/>
+      <c r="E3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="14"/>
-      <c r="E3" s="12" t="s">
+      <c r="F3" s="10">
+        <v>1</v>
+      </c>
+      <c r="G3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="12">
-        <v>1</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" s="15"/>
+      <c r="H3" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="13"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="11">
+      <c r="A4" s="9">
         <v>102</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="15" t="s">
+      <c r="B4" s="10">
+        <v>1</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="12"/>
+      <c r="E4" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="10">
+        <v>1</v>
+      </c>
+      <c r="G4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="14"/>
-      <c r="E4" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="12">
-        <v>1</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="I4" s="17"/>
+      <c r="H4" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="15"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="11">
+      <c r="A5" s="9">
         <v>103</v>
       </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="15" t="s">
+      <c r="B5" s="10">
+        <v>1</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="12"/>
+      <c r="E5" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="10">
+        <v>1</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="14"/>
-      <c r="E5" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="12">
-        <v>1</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="I5" s="15"/>
+      <c r="I5" s="13"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="11">
+      <c r="A6" s="9">
         <v>104</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="15" t="s">
+      <c r="B6" s="10">
+        <v>1</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="12"/>
+      <c r="E6" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="10">
+        <v>1</v>
+      </c>
+      <c r="G6" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="14"/>
-      <c r="E6" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="12">
-        <v>1</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="I6" s="17"/>
+      <c r="H6" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" s="15"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="11">
+      <c r="A7" s="9">
         <v>105</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="15" t="s">
+      <c r="B7" s="10">
+        <v>1</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="12"/>
+      <c r="E7" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="10">
+        <v>1</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" s="17" t="s">
         <v>18</v>
-      </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="12">
-        <v>1</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="I7" s="19" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="11">
+      <c r="A8" s="9">
         <v>106</v>
       </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="12">
-        <v>1</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" s="15"/>
-      <c r="I8" s="17"/>
+      <c r="B8" s="10">
+        <v>1</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="12"/>
+      <c r="E8" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="10">
+        <v>1</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="13"/>
+      <c r="I8" s="15"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="11">
+      <c r="A9" s="9">
         <v>107</v>
       </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="15" t="s">
+      <c r="B9" s="10">
+        <v>1</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="12"/>
+      <c r="E9" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="10">
+        <v>1</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="14"/>
-      <c r="E9" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="12">
-        <v>1</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="H9" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="I9" s="17"/>
+      <c r="I9" s="15"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C2">
@@ -857,7 +876,7 @@
     <cfRule type="duplicateValues" dxfId="0" priority="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Will & Michael - #1140935 We made it so that "shared teams/coaches" will not only play at different times but also will not play each other.
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
   <si>
     <t>TEAM  LIST  AS  OF :</t>
   </si>
@@ -70,9 +70,6 @@
   </si>
   <si>
     <t>105-IRISH-WEBSTER 1</t>
-  </si>
-  <si>
-    <t>Irish 2, Bears 3</t>
   </si>
   <si>
     <t>106-PATRIOTS</t>
@@ -635,7 +632,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -666,10 +663,10 @@
     </row>
     <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="18" t="s">
         <v>26</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>27</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>1</v>
@@ -714,7 +711,7 @@
         <v>10</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I3" s="13"/>
     </row>
@@ -739,7 +736,7 @@
         <v>12</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I4" s="15"/>
     </row>
@@ -789,7 +786,7 @@
         <v>16</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I6" s="15"/>
     </row>
@@ -814,10 +811,10 @@
         <v>10</v>
       </c>
       <c r="H7" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="I7" s="17" t="s">
-        <v>18</v>
+        <v>23</v>
+      </c>
+      <c r="I7" s="17">
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -828,7 +825,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="10" t="s">
@@ -851,7 +848,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="10" t="s">
@@ -864,7 +861,7 @@
         <v>12</v>
       </c>
       <c r="H9" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I9" s="15"/>
     </row>

</xml_diff>